<commit_message>
updated Main and funcitons
Changed main and functions to be compatible with the config file and to account for initial dropped points. Removed some output graphs. Changed graph output to .svg
</commit_message>
<xml_diff>
--- a/Data/Program output/All posts.xlsx
+++ b/Data/Program output/All posts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dispe\Code\Dual-Deflection\Data\Program output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b08f9f412f899893/Documents/GitHub/dual_deflection/Data/Program output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5BC00F5-58FD-4D96-B578-01E98CA696E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{D5BC00F5-58FD-4D96-B578-01E98CA696E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B7ABDAB-EFAD-4099-A432-9E2E2F6EC3B3}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25815" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26820" yWindow="0" windowWidth="24780" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -545,6 +545,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="14" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>